<commit_message>
adicionada interface raiz 'report' em biblioteca CRISPDM(objetiva a criação de funções que ajudem a automatizar a unificação dos dados, a medida que ajuda o ser humano a visualizar os dados); Adicionada função cria_hash_nomesTabelas_nomesColuna de nome auto-explicativo
</commit_message>
<xml_diff>
--- a/quantidade_para_cada_observacao.xlsx
+++ b/quantidade_para_cada_observacao.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>observacoes</t>
   </si>
@@ -29,13 +29,19 @@
     <t>3</t>
   </si>
   <si>
-    <t>1935</t>
+    <t>4</t>
   </si>
   <si>
-    <t>1995</t>
+    <t>2016</t>
   </si>
   <si>
-    <t>1996</t>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2106</t>
+  </si>
+  <si>
+    <t>2916</t>
   </si>
 </sst>
 </file>
@@ -100,10 +106,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>1484258.0</v>
       </c>
     </row>
     <row r="3">
@@ -111,10 +117,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>701.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -122,10 +128,21 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>13.0</v>
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>